<commit_message>
Cleared formatting from the title column
</commit_message>
<xml_diff>
--- a/excel-to-dsc_Yale-Template.xlsx
+++ b/excel-to-dsc_Yale-Template.xlsx
@@ -1870,7 +1870,7 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2029,26 +2029,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="54"/>
       <name val="Calibri"/>
@@ -2057,12 +2037,6 @@
     <font>
       <sz val="14"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFED7D31"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2414,7 +2388,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2429,27 +2403,18 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2458,26 +2423,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2818,7 +2765,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3036,11 +2983,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="11"/>
+      <c r="D2"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
@@ -3058,9 +3005,9 @@
       <c r="X2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
-      <c r="AE2" s="12"/>
+      <c r="AE2" s="10"/>
       <c r="AF2" s="5"/>
-      <c r="AG2" s="14"/>
+      <c r="AG2" s="12"/>
       <c r="AH2" s="5"/>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
@@ -3079,230 +3026,227 @@
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
       <c r="AY2" s="5"/>
-      <c r="AZ2" s="15"/>
-    </row>
-    <row r="3" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="4" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-    </row>
-    <row r="5" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="19"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="24"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-    </row>
-    <row r="8" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="25"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-    </row>
-    <row r="9" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="20"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-    </row>
-    <row r="10" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="21"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-    </row>
-    <row r="11" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="21"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-    </row>
-    <row r="12" spans="1:55" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="21"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="AG12" s="22"/>
-    </row>
-    <row r="13" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="20"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-    </row>
-    <row r="14" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="23"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
+      <c r="AZ2" s="13"/>
+    </row>
+    <row r="3" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+    </row>
+    <row r="4" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+    </row>
+    <row r="5" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D5"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+    </row>
+    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+    </row>
+    <row r="8" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D11"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+    </row>
+    <row r="12" spans="1:55" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D12"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="AG12" s="16"/>
+    </row>
+    <row r="13" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+    </row>
+    <row r="14" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
     </row>
     <row r="15" spans="1:55" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="1:55" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AG19" s="2"/>
     </row>
-    <row r="20" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AG22" s="2"/>
     </row>
-    <row r="23" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
     </row>
-    <row r="27" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="4:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="33:33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="33:33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="33:33" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed formatting from Scope and Contents column
</commit_message>
<xml_diff>
--- a/excel-to-dsc_Yale-Template.xlsx
+++ b/excel-to-dsc_Yale-Template.xlsx
@@ -1870,7 +1870,7 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2031,18 +2031,6 @@
     <font>
       <sz val="11"/>
       <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2388,7 +2376,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2397,22 +2385,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2765,7 +2741,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2983,37 +2959,46 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+    <row r="2" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
       <c r="D2"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="V2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="5"/>
@@ -3026,202 +3011,228 @@
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
       <c r="AY2" s="5"/>
-      <c r="AZ2" s="13"/>
-    </row>
-    <row r="3" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ2" s="9"/>
+    </row>
+    <row r="3" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
       <c r="D3"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-    </row>
-    <row r="4" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+    </row>
+    <row r="4" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-    </row>
-    <row r="5" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-    </row>
-    <row r="6" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-    </row>
-    <row r="8" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-    </row>
-    <row r="9" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-    </row>
-    <row r="10" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-    </row>
-    <row r="11" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-    </row>
-    <row r="12" spans="1:55" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:55" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D12"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="AG12" s="16"/>
-    </row>
-    <row r="13" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="AG12" s="12"/>
+    </row>
+    <row r="13" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-    </row>
-    <row r="14" spans="1:55" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:55" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:55" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:55" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="33:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3652,7 +3663,7 @@
     <row r="383" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="384" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A4:A1048576 A1">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="1"/>
@@ -3726,7 +3737,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A4:A1048576 A1</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
fixed controlaccess column for single values
</commit_message>
<xml_diff>
--- a/excel-to-dsc_Yale-Template.xlsx
+++ b/excel-to-dsc_Yale-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mc2343\Documents\GitHub\Excel-to-DSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mc2343\Documents\ins-and-outs-of-ArchivesSpace\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2741,7 +2741,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3663,7 +3663,7 @@
     <row r="383" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="384" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A4:A1048576 A1">
+  <conditionalFormatting sqref="A2:A1048576 A1">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="1"/>
@@ -3737,7 +3737,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A4:A1048576 A1</xm:sqref>
+          <xm:sqref>A2:A1048576 A1</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
adding duration, page, and item_barcode to the dropdown options
</commit_message>
<xml_diff>
--- a/excel-to-dsc_Yale-Template.xlsx
+++ b/excel-to-dsc_Yale-Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mc2343\Documents\ins-and-outs-of-ArchivesSpace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mc2343\Documents\GitHub\Excel-to-DSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,13 +29,13 @@
     <definedName name="container_2_type">ContainerList!$W:$W</definedName>
     <definedName name="container_3_type">ContainerList!$Y:$Y</definedName>
     <definedName name="container_profile">ContainerList!$T:$T</definedName>
-    <definedName name="ContainerValues">ControlledVocab!$C$2:$C$10</definedName>
+    <definedName name="ContainerValues">ControlledVocab!$C$2:$C$12</definedName>
     <definedName name="date_expression">ContainerList!$E:$E</definedName>
     <definedName name="day_begin">ContainerList!$H:$H</definedName>
     <definedName name="day_end">ContainerList!$K:$K</definedName>
     <definedName name="extent_number">ContainerList!$AA:$AA</definedName>
     <definedName name="extent_value">ContainerList!$AB:$AB</definedName>
-    <definedName name="ExtentValues">ControlledVocab!$D$2:$D$36</definedName>
+    <definedName name="ExtentValues">ControlledVocab!$D$2:$D$37</definedName>
     <definedName name="generic_extent">ContainerList!$AC:$AC</definedName>
     <definedName name="instance_type">ContainerList!$R:$R</definedName>
     <definedName name="InstanceValues">ControlledVocab!$B$2:$B$11</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="606">
   <si>
     <t>level number</t>
   </si>
@@ -1860,12 +1860,21 @@
   </si>
   <si>
     <t>zza - Zaza; Dimili; Dimli; Kirdki; Kirmanjki; Zazaki</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>item_barcode</t>
+  </si>
+  <si>
+    <t>Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="00"/>
@@ -2741,7 +2750,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2764,11 +2773,11 @@
     <col min="18" max="18" width="13.28515625" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="16.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="21" max="21" width="24.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="22.85546875" customWidth="1"/>
     <col min="23" max="23" width="16.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="24" max="24" width="23.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="16.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="19" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="16.140625" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="19" customWidth="1" outlineLevel="1"/>
     <col min="27" max="29" width="19" customWidth="1"/>
     <col min="30" max="32" width="19" hidden="1" customWidth="1"/>
     <col min="33" max="34" width="32.42578125" customWidth="1"/>
@@ -3751,7 +3760,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3759,7 +3768,7 @@
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="74.140625" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
@@ -3923,6 +3932,9 @@
       <c r="B11" t="s">
         <v>91</v>
       </c>
+      <c r="C11" t="s">
+        <v>605</v>
+      </c>
       <c r="D11" t="s">
         <v>92</v>
       </c>
@@ -3931,6 +3943,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>604</v>
+      </c>
       <c r="D12" t="s">
         <v>93</v>
       </c>
@@ -4131,6 +4146,9 @@
       </c>
     </row>
     <row r="37" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>603</v>
+      </c>
       <c r="E37" t="s">
         <v>153</v>
       </c>

</xml_diff>